<commit_message>
release dak-pnc 1.0.0 and pcmt-vax-prequal 0.2.0
</commit_message>
<xml_diff>
--- a/pcmt-vaxprequal/CodeSystem-PreQualPresentation.xlsx
+++ b/pcmt-vaxprequal/CodeSystem-PreQualPresentation.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-01T08:33:29+00:00</t>
+    <t>2025-09-16T20:42:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>